<commit_message>
Create AccesoryRequest, Create Accessory CRUD Method, Create Accessory import, Fix Costume Model to Accessories typo, Add status column on Costume and Accessory
</commit_message>
<xml_diff>
--- a/public/cost.xlsx
+++ b/public/cost.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="100">
   <si>
     <t>Keqing Cheongsam</t>
   </si>
@@ -318,6 +318,12 @@
   </si>
   <si>
     <t>2B Nier</t>
+  </si>
+  <si>
+    <t>Ishtar Maid Ver</t>
+  </si>
+  <si>
+    <t>Kotori Police</t>
   </si>
 </sst>
 </file>
@@ -635,13 +641,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -2443,6 +2452,46 @@
         <v>80000</v>
       </c>
     </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>98</v>
+      </c>
+      <c r="B91">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>90</v>
+      </c>
+      <c r="E91">
+        <v>70</v>
+      </c>
+      <c r="F91">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>99</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>90</v>
+      </c>
+      <c r="E92">
+        <v>70</v>
+      </c>
+      <c r="F92">
+        <v>70000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>